<commit_message>
Maintainance test functions to RW
</commit_message>
<xml_diff>
--- a/Parts - Consoles.csv.xlsx
+++ b/Parts - Consoles.csv.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="96">
   <si>
     <t>RecordID</t>
   </si>
@@ -114,6 +114,9 @@
     <t>Test Mode Image</t>
   </si>
   <si>
+    <t>Incline Calibration</t>
+  </si>
+  <si>
     <t>Display Test</t>
   </si>
   <si>
@@ -123,7 +126,7 @@
     <t>Button Test</t>
   </si>
   <si>
-    <t>Button TestImage</t>
+    <t>Button Test Image</t>
   </si>
   <si>
     <t>Drive Motor Output Test</t>
@@ -169,9 +172,6 @@
   </si>
   <si>
     <t>Updated</t>
-  </si>
-  <si>
-    <t>Created</t>
   </si>
   <si>
     <t>385843</t>
@@ -223,6 +223,25 @@
     <t>Insert Dead Man Key into console.</t>
   </si>
   <si>
+    <t>Touch user profile icon at the lower right  of the screen
+Touch settings
+Touch “Equipment Info” and then “App Info”. This will display App version and Brainboard version.
+Verify and Record.
+Press the back arrow on the tablet to return to main screen</t>
+  </si>
+  <si>
+    <t>Touch the user profile icon on lower right of the screen
+Touch Settings
+Touch Maintainance
+Select Calibrate Incline
+Press Calibrate on EQF1259
+Press Begin on tablet to start incline calibration.  Verify the incline value on the display increases briefly, pauses, then decrease to zero
+When calibration is complete, press the back arrow on the tablet to return to main screen</t>
+  </si>
+  <si>
+    <t>Verify tablet display is lit and without flaws</t>
+  </si>
+  <si>
     <t>On the console, press random Quick speed buttons.
 Verify that the Speed on the console and EQF1259 match.</t>
   </si>
@@ -262,7 +281,7 @@
 Disconnect all wires and cables from the console.</t>
   </si>
   <si>
-    <t>PIP Generator</t>
+    <t>PIP_GEN_ID-0</t>
   </si>
   <si>
     <t>REV 0</t>
@@ -274,7 +293,7 @@
     <t>From chaos, springs new beginnings!</t>
   </si>
   <si>
-    <t>ID_0</t>
+    <t>id-0</t>
   </si>
   <si>
     <t>REV 1</t>
@@ -283,7 +302,7 @@
     <t>20171205</t>
   </si>
   <si>
-    <t>Created arrays to add functionality for individual variables</t>
+    <t>Created arrays for variables</t>
   </si>
   <si>
     <t>REV 2</t>
@@ -292,7 +311,7 @@
     <t>20171206</t>
   </si>
   <si>
-    <t>Added time stamping and found no use but will leave in</t>
+    <t>Added time stamping</t>
   </si>
   <si>
     <t>REV 3</t>
@@ -310,16 +329,19 @@
     <t>20171227</t>
   </si>
   <si>
-    <t>Converted to openpyxl and functions on test x.xml</t>
+    <t>Converted to openpyxl</t>
+  </si>
+  <si>
+    <t>REV 5</t>
+  </si>
+  <si>
+    <t>20180112</t>
+  </si>
+  <si>
+    <t>Killed trackvia full table</t>
   </si>
   <si>
     <t>REV</t>
-  </si>
-  <si>
-    <t>20180112</t>
-  </si>
-  <si>
-    <t>Killed trackvia full table and will upload individual as created</t>
   </si>
   <si>
     <t>Let justice be done, though the heavens fall!</t>
@@ -915,35 +937,47 @@
       <c r="AA2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="AH2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="AO2" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AQ2" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AR2" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="AS2" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="AV2" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AX2" t="s">
-        <v>71</v>
+        <v>74</v>
+      </c>
+      <c r="AZ2" s="2" t="n">
+        <v>43119.5863994213</v>
       </c>
     </row>
   </sheetData>
@@ -967,106 +1001,106 @@
   <cols>
     <col customWidth="1" max="1" min="1" width="8.4"/>
     <col customWidth="1" max="2" min="2" width="12"/>
-    <col customWidth="1" max="3" min="3" width="79.2"/>
+    <col customWidth="1" max="3" min="3" width="56.4"/>
     <col customWidth="1" max="4" min="4" width="7.199999999999999"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" t="s">
         <v>78</v>
-      </c>
-      <c r="D2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>43119.45376019676</v>
+        <v>43119.5863697338</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>